<commit_message>
added many IPExtension edit Methods
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998B9E4D-A0D0-468B-8FC6-9CF7EDDE9D43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B111668-69DC-4907-B82F-D2DC3B141362}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -169,6 +169,36 @@
   </si>
   <si>
     <t>number_initiate -number 90000..90001 -numbertype ex,90000-90001,90000,1,FirstName,LastName,Mitel 6869i,Mitel 6873i,ip_extension -e -d 90000,extension -e -d 90000,number_end -number 90000..90001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 90000..90001 -numbertype ex,90000-90001,90000,1,FirstName,LastName,Mitel 6869i,ip_extension -e -d 90000,extension -e -d 90000,number_end -number 90000..90001 -numbertype ex,1 - CSP 1</t>
+  </si>
+  <si>
+    <t>test_editIPExtensionCSP</t>
+  </si>
+  <si>
+    <t>number_initiate -number 90000..90001 -numbertype ex,90000-90001,90000,1,FirstName,LastName,Mitel 6869i,ip_extension -e -d 90000,extension -e -d 90000,number_end -number 90000..90001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_editToAssignThirdPartySIPClient</t>
+  </si>
+  <si>
+    <t>test_editToConfigureCallPark</t>
+  </si>
+  <si>
+    <t>test_editToConfigureSecondLineState</t>
+  </si>
+  <si>
+    <t>test_editToConfigureHotLineNumber</t>
+  </si>
+  <si>
+    <t>number_initiate -number 70001..70002 -numbertype ex,extension -i -d 70001..70002 -l 1 --csp 0,ip_extension -i -d 70001..70002,70001,70002,ip_extension -e -d 70001..70002,extension -e -d 70001..70002,number_end -number 70001..70002 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_editToSetFirst_LastNames</t>
+  </si>
+  <si>
+    <t>number_initiate -number 70001..70002 -numbertype ex,extension -i -d 70001..70002 -l 1 --csp 0,ip_extension -i -d 70001..70002,70001,EditedFirstName,EditedLastName,ip_extension -e -d 70001..70002,extension -e -d 70001..70002,number_end -number 70001..70002 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -617,10 +647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -813,8 +843,71 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
+    <row r="18" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added dmn function key test
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B111668-69DC-4907-B82F-D2DC3B141362}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD964F00-E9F8-432E-9642-1933EB6AB6FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -199,6 +199,17 @@
   </si>
   <si>
     <t>number_initiate -number 70001..70002 -numbertype ex,extension -i -d 70001..70002 -l 1 --csp 0,ip_extension -i -d 70001..70002,70001,EditedFirstName,EditedLastName,ip_extension -e -d 70001..70002,extension -e -d 70001..70002,number_end -number 70001..70002 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_createDMN_FuncKey</t>
+  </si>
+  <si>
+    <t>number_initiate -number 60000 -numbertype ex,
+extension -i -d 60000 -l 1 --csp 0,
+ip_extension -i -d 60000</t>
+  </si>
+  <si>
+    <t>number_initiate -number 90000 -numbertype ex,90000,90000,60000,1,FirstName,LastName,Mitel 6869i,DMN,ip_extension -e -d 60000..90000,extension -e -d 60000..90000,number_end -number 60000 -numbertype ex,number_end -number 90000 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -647,16 +658,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.08984375" customWidth="1"/>
+    <col min="4" max="4" width="108.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -832,7 +844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -843,7 +855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -854,7 +866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -865,7 +877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -876,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -887,7 +899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -898,7 +910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -907,6 +919,20 @@
       </c>
       <c r="C23" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added FunctionKeys remove methods
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7AE305-D053-4E47-81C4-C442DFF2AE00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104AF887-A49E-48C2-9EA1-321A095A335D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="98">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -273,6 +273,60 @@
   </si>
   <si>
     <t>number_initiate -number 10001 -numbertype ex,10001,10001,1,FirstName,LastName,Mitel 6869i,ip_extension -e -d 10001,extension -e -d 10001,number_end -number 10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_clearTNS_funcKey</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function TNS --display-text "TNS-10001" --key 1 --key-sequence 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_clearMNS_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearEDN_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearMOI_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearPGM_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearREC_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearDMN_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearGMA_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearMCT_funcKey</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function MNS --display-text "MNS-10001" --key 1 --monitored-dir 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function EDN --display-text "EDN-10001" --key 1 --line-dir 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function XML --display-text "MOI" --key 1 --xml-on-demand-uri http://$$PROXYURL$$:22222/StreamingMenu?user=$$SIPUSERNAME$$,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function PGM --display-text "PGM" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function REC --display-text "REC" --key 1 --record-on-demand-uri 'http://149.13.0.80:80//nrj.ogg',10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function DMN --display-text "DMN-10001" --key 1 --monitored-dir 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function GMA --display-text "GMA-10001" --key 1 --monitored-dir 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function MCT --display-text "MCT" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -721,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1128,6 +1182,106 @@
       </c>
       <c r="D34" s="2" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sca_scabr clear tests.
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104AF887-A49E-48C2-9EA1-321A095A335D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2384F32-E142-48FF-B969-63BA28478EF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -327,6 +327,18 @@
   </si>
   <si>
     <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function MCT --display-text "MCT" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_clearSCA_funcKey</t>
+  </si>
+  <si>
+    <t>test_clearSCABR_funcKey</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function SCA --display-text "SCA" --line 1 --line-dir 10000,extension_key -i --dir 10001 --function SCA --display-text "SCA" --key 1 --line-dir 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function SCABR --display-text "SCABR" --line 1 --line-dir 10000,extension_key -i --dir 10001 --function SCABR --display-text "SCABR" --key 1 --line-dir 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -775,10 +787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1281,6 +1293,28 @@
         <v>97</v>
       </c>
       <c r="C43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Digital extension classes
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2384F32-E142-48FF-B969-63BA28478EF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2A1CE0-7A2E-4947-9734-761FA4C75814}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
-  <si>
-    <t>Arjuna,Arjuna@12345</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="130">
   <si>
     <t>TestCase</t>
   </si>
@@ -154,12 +151,6 @@
   </si>
   <si>
     <t>test_editIPExtensionPhoneType</t>
-  </si>
-  <si>
-    <t>http://10.211.162.113/mp</t>
-  </si>
-  <si>
-    <t>http://10.211.162.113/wbm</t>
   </si>
   <si>
     <t>number_initiate -number 90000..90001 -numbertype ex,90000-90001,90000,1,FirstName,LastName,Mitel 6869i,Mitel 6873i,ip_extension -e -d 90000,extension -e -d 90000,number_end -number 90000..90001 -numbertype ex</t>
@@ -278,9 +269,6 @@
     <t>test_clearTNS_funcKey</t>
   </si>
   <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function TNS --display-text "TNS-10001" --key 1 --key-sequence 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
     <t>test_clearMNS_funcKey</t>
   </si>
   <si>
@@ -305,40 +293,136 @@
     <t>test_clearMCT_funcKey</t>
   </si>
   <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function MNS --display-text "MNS-10001" --key 1 --monitored-dir 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function EDN --display-text "EDN-10001" --key 1 --line-dir 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function XML --display-text "MOI" --key 1 --xml-on-demand-uri http://$$PROXYURL$$:22222/StreamingMenu?user=$$SIPUSERNAME$$,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function PGM --display-text "PGM" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function REC --display-text "REC" --key 1 --record-on-demand-uri 'http://149.13.0.80:80//nrj.ogg',10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function DMN --display-text "DMN-10001" --key 1 --monitored-dir 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function GMA --display-text "GMA-10001" --key 1 --monitored-dir 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function MCT --display-text "MCT" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
     <t>test_clearSCA_funcKey</t>
   </si>
   <si>
     <t>test_clearSCABR_funcKey</t>
   </si>
   <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function SCA --display-text "SCA" --line 1 --line-dir 10000,extension_key -i --dir 10001 --function SCA --display-text "SCA" --key 1 --line-dir 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --dir 10000 --function SCABR --display-text "SCABR" --line 1 --line-dir 10000,extension_key -i --dir 10001 --function SCABR --display-text "SCABR" --key 1 --line-dir 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+    <t>test_create_all_function_keys</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000..80005 -numbertype ex,extension -i -d 80000..80005 -l 1 --csp 0,ip_extension -i -d 80000..80005,80000,80001,80002,80003,80004</t>
+  </si>
+  <si>
+    <t>test_createUserWithExtension</t>
+  </si>
+  <si>
+    <t>test_editUserToRemoveExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000 -numbertype ex,extension -i -d 10000 -l 1 --csp 0,ip_extension -i -d 10000,10000,ip_extension -e -d 10000,extension -e -d 10000,number_end -number 10000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_editUserAssignExistingExtension</t>
+  </si>
+  <si>
+    <t>test_createUserAssignExistingExtension</t>
+  </si>
+  <si>
+    <t>test_createUserWithExtesnsionUsingIPTemplate</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000 -numbertype ex,10000,IPTemp,Mitel 6869i,ip_extension -e -d 10000,extension -e -d 10000,number_end -number 10000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_IP_extension_usingTemplate</t>
+  </si>
+  <si>
+    <t>test_editUserAssignNewExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000 -numbertype ex,10000,Mitel 6869i,ip_extension -e -d 10000,extension -e -d 10000,number_end -number 10000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_createAnalogExtension</t>
+  </si>
+  <si>
+    <t>test_createDigitalExtension</t>
+  </si>
+  <si>
+    <t>test_edit_digital_extension_toChange_CAT</t>
+  </si>
+  <si>
+    <t>test_edit_digital_extension_toChange_First_Last_Names</t>
+  </si>
+  <si>
+    <t>test_edit_digital_extension_toChange_PhoneModel</t>
+  </si>
+  <si>
+    <t>test_edit_digital_extension_toSet_AgentPosition</t>
+  </si>
+  <si>
+    <t>number_initiate -number 90000000000000000000 -numbertype ex,extension -i -d 90000000000000000000 -l 1 --csp 0,ip_extension -i -d 90000000000000000000,90000000000000000000,ip_extension -e -d 90000000000000000000,extension -e -d 90000000000000000000,number_end -number 90000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_digital_extension_toSet_HotLine</t>
+  </si>
+  <si>
+    <t>Arjuna,Arjuna@12345</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function TNS --display-text "TNS-10001" --key 1 --key-sequence 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function MNS --display-text "MNS-10001" --key 1 --monitored-DIR 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function EDN --display-text "EDN-10001" --key 1 --line-DIR 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function XML --display-text "MOI" --key 1 --xml-on-demand-uri http://$$PROXYURL$$:22222/StreamingMenu?user=$$SIPUSERNAME$$,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function PGM --display-text "PGM" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function REC --display-text "REC" --key 1 --record-on-demand-uri 'http://149.13.0.80:80//nrj.ogg',10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function DMN --display-text "DMN-10001" --key 1 --monitored-DIR 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function GMA --display-text "GMA-10001" --key 1 --monitored-DIR 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function MCT --display-text "MCT" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function SCA --display-text "SCA" --line 1 --line-DIR 10000,extension_key -i --DIR 10001 --function SCA --display-text "SCA" --key 1 --line-DIR 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function SCABR --display-text "SCABR" --line 1 --line-DIR 10000,extension_key -i --DIR 10001 --function SCABR --display-text "SCABR" --key 1 --line-DIR 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000 -numbertype ex,10000,1,FirstName,LastName,MiVoice 4220 (DBC220),KSEXE:DIR=19001;,number_end -number 10000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,MiVoice 4225 (DBC225),1B-2-20-00,FirstName,LastName,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,MiVoice 4222 (DBC222),KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_digital_extension_toDelayed_HotLine</t>
+  </si>
+  <si>
+    <t>test_delete_digitalExtension</t>
+  </si>
+  <si>
+    <t>test_swap_digitalEquipmentPositions</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000..80000000000000000001 -numbertype ex,80000000000000000000,1B-2-20-00,80000000000000000001,1B-2-20-01,KSEXE:DIR=80000000000000000000;,KSEXE:DIR=80000000000000000001;,number_end -number 80000000000000000000..80000000000000000001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>https://10.211.62.216/mp</t>
+  </si>
+  <si>
+    <t>https://10.211.62.214/wbm</t>
   </si>
 </sst>
 </file>
@@ -671,7 +755,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -682,101 +766,101 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -787,535 +871,758 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.08984375" customWidth="1"/>
-    <col min="4" max="4" width="108.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="2" t="s">
+    </row>
+    <row r="54" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>101</v>
       </c>
-      <c r="C45" t="s">
-        <v>5</v>
+      <c r="B55" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1339,13 +1646,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1364,7 +1671,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1374,12 +1681,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all analog test methods
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F857D59D-C2E0-4ADB-A02B-FF15D1E9F5FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2ECB67-1EE8-4C35-BCDB-FD82B7883FC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="158">
   <si>
     <t>TestCase</t>
   </si>
@@ -395,9 +395,6 @@
     <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function SCABR --display-text "SCABR" --line 1 --line-DIR 10000,extension_key -i --DIR 10001 --function SCABR --display-text "SCABR" --key 1 --line-DIR 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
   </si>
   <si>
-    <t>number_initiate -number 10000 -numbertype ex,10000,1,FirstName,LastName,MiVoice 4220 (DBC220),KSEXE:DIR=19001;,number_end -number 10000 -numbertype ex</t>
-  </si>
-  <si>
     <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,MiVoice 4225 (DBC225),1B-2-20-00,FirstName,LastName,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
   </si>
   <si>
@@ -453,6 +450,63 @@
   </si>
   <si>
     <t>test_editUser_to_create_DigitalExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,FirstName,LastName,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toChange_CAT</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toChange_First_Last_Names</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_equipmentPosition</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,1B-2-10-01,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toSet_HotLine</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toDelayed_HotLine</t>
+  </si>
+  <si>
+    <t>test_delete_analogExtension</t>
+  </si>
+  <si>
+    <t>test_swap_analogEquipmentPositions</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000..80000000000000000001 -numbertype ex,80000000000000000000,1B-2-10-00,80000000000000000001,1B-2-10-01,EXTEE:DIR=80000000000000000000;,EXTEE:DIR=80000000000000000001;,number_end -number 80000000000000000000..80000000000000000001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_analogExt_using_Template</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,AnalogTemplate,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_createUser_with_analog_Extension</t>
+  </si>
+  <si>
+    <t>test_createUser_with_existing_analog_Extension</t>
+  </si>
+  <si>
+    <t>test_createUser_with_AnalogExtension_usingTemplate</t>
+  </si>
+  <si>
+    <t>test_editUser_and_Assign_Existing_AnalogExtension</t>
+  </si>
+  <si>
+    <t>test_editUser_and_remove_Existing_AnalogExtension</t>
+  </si>
+  <si>
+    <t>test_editUser_to_create_AnalogExtension</t>
   </si>
 </sst>
 </file>
@@ -901,10 +955,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1468,7 +1522,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -1540,7 +1594,7 @@
     </row>
     <row r="54" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>120</v>
@@ -1551,7 +1605,7 @@
     </row>
     <row r="55" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>121</v>
@@ -1562,10 +1616,10 @@
     </row>
     <row r="56" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -1573,10 +1627,10 @@
     </row>
     <row r="57" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -1584,33 +1638,36 @@
     </row>
     <row r="58" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -1619,37 +1676,34 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>124</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>125</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -1657,16 +1711,19 @@
     </row>
     <row r="64" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="D64" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>132</v>
       </c>
@@ -1680,7 +1737,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -1691,10 +1748,10 @@
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -1705,10 +1762,10 @@
         <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -1719,35 +1776,210 @@
         <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C69" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C70" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>137</v>
+    </row>
+    <row r="71" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>147</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>148</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>152</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>153</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>156</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1806,12 +2038,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Personal number tests for few extensions...
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48856F6-D257-42AC-BDBE-CCB4E063E094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75417A5A-9089-4CE3-A978-23292429E14B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="225">
   <si>
     <t>TestCase</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>test_snm_invalidUserID_login</t>
-  </si>
-  <si>
-    <t>mxone_admin,Mxone@456</t>
   </si>
   <si>
     <t>Mxone@456</t>
@@ -359,250 +356,362 @@
     <t>test_edit_digital_extension_toSet_HotLine</t>
   </si>
   <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function TNS --display-text "TNS-10001" --key 1 --key-sequence 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function MNS --display-text "MNS-10001" --key 1 --monitored-DIR 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function EDN --display-text "EDN-10001" --key 1 --line-DIR 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function XML --display-text "MOI" --key 1 --xml-on-demand-uri http://$$PROXYURL$$:22222/StreamingMenu?user=$$SIPUSERNAME$$,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function PGM --display-text "PGM" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function REC --display-text "REC" --key 1 --record-on-demand-uri 'http://149.13.0.80:80//nrj.ogg',10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function DMN --display-text "DMN-10001" --key 1 --monitored-DIR 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function GMA --display-text "GMA-10001" --key 1 --monitored-DIR 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function MCT --display-text "MCT" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function SCA --display-text "SCA" --line 1 --line-DIR 10000,extension_key -i --DIR 10001 --function SCA --display-text "SCA" --key 1 --line-DIR 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function SCABR --display-text "SCABR" --line 1 --line-DIR 10000,extension_key -i --DIR 10001 --function SCABR --display-text "SCABR" --key 1 --line-DIR 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,MiVoice 4225 (DBC225),1B-2-20-00,FirstName,LastName,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,MiVoice 4222 (DBC222),KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_digital_extension_toDelayed_HotLine</t>
+  </si>
+  <si>
+    <t>test_delete_digitalExtension</t>
+  </si>
+  <si>
+    <t>test_swap_digitalEquipmentPositions</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000..80000000000000000001 -numbertype ex,80000000000000000000,1B-2-20-00,80000000000000000001,1B-2-20-01,KSEXE:DIR=80000000000000000000;,KSEXE:DIR=80000000000000000001;,number_end -number 80000000000000000000..80000000000000000001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_digitalExt_using_Template</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,DigitalTemplate,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_createUser_with_Digital_Extension</t>
+  </si>
+  <si>
+    <t>test_createUser_with_existing_Digital_Extension</t>
+  </si>
+  <si>
+    <t>test_createUser_with_DigitalExtension_usingTemplate</t>
+  </si>
+  <si>
+    <t>test_editUser_and_Assign_Existing_DigitalExtension</t>
+  </si>
+  <si>
+    <t>test_editUser_and_remove_Existing_DigitalExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,MiVoice 4225 (DBC225),1B-2-20-00,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,80000000000000000000,1,FirstName,LastName,Mitel 6869i,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_editUser_to_create_DigitalExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,FirstName,LastName,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toChange_CAT</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toChange_First_Last_Names</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_equipmentPosition</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,1B-2-10-01,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toSet_HotLine</t>
+  </si>
+  <si>
+    <t>test_edit_analog_extension_toDelayed_HotLine</t>
+  </si>
+  <si>
+    <t>test_delete_analogExtension</t>
+  </si>
+  <si>
+    <t>test_swap_analogEquipmentPositions</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000..80000000000000000001 -numbertype ex,80000000000000000000,1B-2-10-00,80000000000000000001,1B-2-10-01,EXTEE:DIR=80000000000000000000;,EXTEE:DIR=80000000000000000001;,number_end -number 80000000000000000000..80000000000000000001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_analogExt_using_Template</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,AnalogTemplate,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_createUser_with_analog_Extension</t>
+  </si>
+  <si>
+    <t>test_createUser_with_existing_analog_Extension</t>
+  </si>
+  <si>
+    <t>test_createUser_with_AnalogExtension_usingTemplate</t>
+  </si>
+  <si>
+    <t>test_editUser_and_Assign_Existing_AnalogExtension</t>
+  </si>
+  <si>
+    <t>test_editUser_and_remove_Existing_AnalogExtension</t>
+  </si>
+  <si>
+    <t>test_editUser_to_create_AnalogExtension</t>
+  </si>
+  <si>
+    <t>test_create_virtual_extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_delete_virtual_extension</t>
+  </si>
+  <si>
+    <t>test_delete_multiple_virtual_extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000001..80000000000000000010 -numbertype ex,extension -i -d 80000000000000000001..80000000000000000010 -l 1 --csp 0,80000000000000000001-80000000000000000010,extension -e -d 80000000000000000001..80000000000000000010,number_end -number 80000000000000000001..80000000000000000010 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_configureParallel_ringing_to_VirtualExt</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000001..80000000000000000003 -numbertype ex,extension -i -d 80000000000000000001..80000000000000000003 -l 1 --csp 0,80000000000000000001-80000000000000000003,80000000000000000001,80000000000000000002,80000000000000000003,parallel_ringing -e -d 80000000000000000001,extension -e -d 80000000000000000001..80000000000000000003,number_end -number 80000000000000000001..80000000000000000003 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_virtual_extension_CSP</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex,1 - CSP 1</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000001..80000000000000000002 -numbertype ex,extension -i -d 80000000000000000001..80000000000000000002 -l 1 --csp 0,80000000000000000001,80000000000000000002,extension -e -d 80000000000000000001..80000000000000000002,number_end -number 80000000000000000001..80000000000000000002 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_editToConfigureHotLineNumber_Virtual</t>
+  </si>
+  <si>
+    <t>test_editToSetFirst_LastNames_virtualExt</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,extension -i -d 80000000000000000000 -l 1 --csp 0,80000000000000000000,EditedFirstName,EditedLastName,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_virtual_extension_usingTemplate</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,VirtualTemplate,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,IPTemp,Mitel 6869i,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_createUser_with_virtualExtension</t>
+  </si>
+  <si>
+    <t>test_editUserToRemove_VirtualExtension</t>
+  </si>
+  <si>
+    <t>test_editUserAssign_Existing_VirtualExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,extension -i -d 80000000000000000000 -l 1 --csp 0,80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_createUserAssign_Existing_VirtualExtension</t>
+  </si>
+  <si>
+    <t>test_createUserWith_Extesnsion_Using_VirtualTemplate</t>
+  </si>
+  <si>
+    <t>test_editUser_Assign_New_VirtualExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,Virtual,Extension,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_multi_terminal_extension</t>
+  </si>
+  <si>
+    <t>test_create_multi_terminal_WithIP</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,parallel_ringing -e -d 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_multi_terminal_WithSIP_Auto</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,65535,roadrunner.com,10.211.62.214,parallel_ringing -e -d 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_multi_terminal_With_MobileExtension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,99999999999999999999</t>
+  </si>
+  <si>
+    <t>https://10.211.62.216/mp</t>
+  </si>
+  <si>
+    <t>https://10.211.62.214/wbm</t>
+  </si>
+  <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
   <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function TNS --display-text "TNS-10001" --key 1 --key-sequence 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function MNS --display-text "MNS-10001" --key 1 --monitored-DIR 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function EDN --display-text "EDN-10001" --key 1 --line-DIR 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function XML --display-text "MOI" --key 1 --xml-on-demand-uri http://$$PROXYURL$$:22222/StreamingMenu?user=$$SIPUSERNAME$$,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function PGM --display-text "PGM" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function REC --display-text "REC" --key 1 --record-on-demand-uri 'http://149.13.0.80:80//nrj.ogg',10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function DMN --display-text "DMN-10001" --key 1 --monitored-DIR 10001 --alert-type 0,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function GMA --display-text "GMA-10001" --key 1 --monitored-DIR 10001,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function MCT --display-text "MCT" --key 1,10000,10001,extension_key -e -d 10000 --key 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function SCA --display-text "SCA" --line 1 --line-DIR 10000,extension_key -i --DIR 10001 --function SCA --display-text "SCA" --key 1 --line-DIR 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 10000..10001 -numbertype ex,extension -i -d 10000..10001 -l 1 --csp 0,ip_extension -i -d 10000..10001,extension_key -i --DIR 10000 --function SCABR --display-text "SCABR" --line 1 --line-DIR 10000,extension_key -i --DIR 10001 --function SCABR --display-text "SCABR" --key 1 --line-DIR 10000,10000,10001,extension_key -e -d 10000 --key 1,extension_key -e -d 10001 --line 1,ip_extension -e -d 10000..10001,extension -e -d 10000..10001,number_end -number 10000..10001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,MiVoice 4225 (DBC225),1B-2-20-00,FirstName,LastName,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,MiVoice 4222 (DBC222),KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_edit_digital_extension_toDelayed_HotLine</t>
-  </si>
-  <si>
-    <t>test_delete_digitalExtension</t>
-  </si>
-  <si>
-    <t>test_swap_digitalEquipmentPositions</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000..80000000000000000001 -numbertype ex,80000000000000000000,1B-2-20-00,80000000000000000001,1B-2-20-01,KSEXE:DIR=80000000000000000000;,KSEXE:DIR=80000000000000000001;,number_end -number 80000000000000000000..80000000000000000001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>https://10.211.62.216/mp</t>
-  </si>
-  <si>
-    <t>https://10.211.62.214/wbm</t>
-  </si>
-  <si>
-    <t>test_create_digitalExt_using_Template</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,DigitalTemplate,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_createUser_with_Digital_Extension</t>
-  </si>
-  <si>
-    <t>test_createUser_with_existing_Digital_Extension</t>
-  </si>
-  <si>
-    <t>test_createUser_with_DigitalExtension_usingTemplate</t>
-  </si>
-  <si>
-    <t>test_editUser_and_Assign_Existing_DigitalExtension</t>
-  </si>
-  <si>
-    <t>test_editUser_and_remove_Existing_DigitalExtension</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,MiVoice 4225 (DBC225),1B-2-20-00,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,80000000000000000000,1,FirstName,LastName,Mitel 6869i,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_editUser_to_create_DigitalExtension</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,FirstName,LastName,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_edit_analog_extension_toChange_CAT</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_edit_analog_extension_toChange_First_Last_Names</t>
-  </si>
-  <si>
-    <t>test_edit_analog_extension_equipmentPosition</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,1B-2-10-01,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_edit_analog_extension_toSet_HotLine</t>
-  </si>
-  <si>
-    <t>test_edit_analog_extension_toDelayed_HotLine</t>
-  </si>
-  <si>
-    <t>test_delete_analogExtension</t>
-  </si>
-  <si>
-    <t>test_swap_analogEquipmentPositions</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000..80000000000000000001 -numbertype ex,80000000000000000000,1B-2-10-00,80000000000000000001,1B-2-10-01,EXTEE:DIR=80000000000000000000;,EXTEE:DIR=80000000000000000001;,number_end -number 80000000000000000000..80000000000000000001 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_create_analogExt_using_Template</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,AnalogTemplate,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_createUser_with_analog_Extension</t>
-  </si>
-  <si>
-    <t>test_createUser_with_existing_analog_Extension</t>
-  </si>
-  <si>
-    <t>test_createUser_with_AnalogExtension_usingTemplate</t>
-  </si>
-  <si>
-    <t>test_editUser_and_Assign_Existing_AnalogExtension</t>
-  </si>
-  <si>
-    <t>test_editUser_and_remove_Existing_AnalogExtension</t>
-  </si>
-  <si>
-    <t>test_editUser_to_create_AnalogExtension</t>
-  </si>
-  <si>
-    <t>test_create_virtual_extension</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_delete_virtual_extension</t>
-  </si>
-  <si>
-    <t>test_delete_multiple_virtual_extension</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000001..80000000000000000010 -numbertype ex,extension -i -d 80000000000000000001..80000000000000000010 -l 1 --csp 0,80000000000000000001-80000000000000000010,extension -e -d 80000000000000000001..80000000000000000010,number_end -number 80000000000000000001..80000000000000000010 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_configureParallel_ringing_to_VirtualExt</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000001..80000000000000000003 -numbertype ex,extension -i -d 80000000000000000001..80000000000000000003 -l 1 --csp 0,80000000000000000001-80000000000000000003,80000000000000000001,80000000000000000002,80000000000000000003,parallel_ringing -e -d 80000000000000000001,extension -e -d 80000000000000000001..80000000000000000003,number_end -number 80000000000000000001..80000000000000000003 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_edit_virtual_extension_CSP</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex,1 - CSP 1</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000001..80000000000000000002 -numbertype ex,extension -i -d 80000000000000000001..80000000000000000002 -l 1 --csp 0,80000000000000000001,80000000000000000002,extension -e -d 80000000000000000001..80000000000000000002,number_end -number 80000000000000000001..80000000000000000002 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_editToConfigureHotLineNumber_Virtual</t>
-  </si>
-  <si>
-    <t>test_editToSetFirst_LastNames_virtualExt</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,extension -i -d 80000000000000000000 -l 1 --csp 0,80000000000000000000,EditedFirstName,EditedLastName,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_create_virtual_extension_usingTemplate</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,VirtualTemplate,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,IPTemp,Mitel 6869i,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_createUser_with_virtualExtension</t>
-  </si>
-  <si>
-    <t>test_editUserToRemove_VirtualExtension</t>
-  </si>
-  <si>
-    <t>test_editUserAssign_Existing_VirtualExtension</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,extension -i -d 80000000000000000000 -l 1 --csp 0,80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_createUserAssign_Existing_VirtualExtension</t>
-  </si>
-  <si>
-    <t>test_createUserWith_Extesnsion_Using_VirtualTemplate</t>
-  </si>
-  <si>
-    <t>test_editUser_Assign_New_VirtualExtension</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,Virtual,Extension,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_create_multi_terminal_extension</t>
-  </si>
-  <si>
-    <t>test_create_multi_terminal_WithIP</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,parallel_ringing -e -d 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_create_multi_terminal_WithSIP_Auto</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,65535,roadrunner.com,10.211.62.214,parallel_ringing -e -d 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>test_create_multi_terminal_With_MobileExtension</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,FirstName,LastName,99999999999999999999</t>
+    <t>mxone_admin,Mxone@456</t>
+  </si>
+  <si>
+    <t>test_create_SIP_DECT_extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,Arjuna,99999,1104100450968,FirstName,LastName,parallel_ringing -e --dir 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_delete_SIPDECT_extension</t>
+  </si>
+  <si>
+    <t>test_delete_multiple_SIPDECT_extension</t>
+  </si>
+  <si>
+    <t>test_edit_configureParallel_ringing_to_SIPDECT</t>
+  </si>
+  <si>
+    <t>number_initiate -number 9000000000..9000000001 -numbertype ex,extension -i -d 9000000000..9000000001
+ -l 1 --csp 0,ip_extension -i -d 9000000000..9000000001,9000000000,9000000001,
+ip_extension -e -d 9000000000..9000000001,extension -e -d 9000000000..9000000001,number_end -number 9000000000..9000000001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_SIPDECT_ExtensionCSP</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,Arjuna,99999,1104100450968,FirstName,LastName,parallel_ringing -e --dir 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex,1 - CSP 1</t>
+  </si>
+  <si>
+    <t>number_initiate -number 90000000000000000000 -numbertype ex,extension -i -d 90000000000000000000
+ -l 1 --csp 0,ip_extension -i -d 90000000000000000000,90000000000000000000,
+ip_extension -e -d 90000000000000000000,extension -e -d 90000000000000000000,number_end -number 90000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_editT_ConfigureHotLineNumber_SIPDECT</t>
+  </si>
+  <si>
+    <t>test_editSet_First_LastNames_SIPDECT</t>
+  </si>
+  <si>
+    <t>test_createUserWith_SIPDECT_Extension</t>
+  </si>
+  <si>
+    <t>test_editUserToRemove_SIPDECT_Extension</t>
+  </si>
+  <si>
+    <t>test_editUser_AssignExisting_SIPDECT_Extension</t>
+  </si>
+  <si>
+    <t>test_createUserAssignExisting_SIPDECT_Extension</t>
+  </si>
+  <si>
+    <t>test_editUserAssignNew_SIPDECT_Extension</t>
+  </si>
+  <si>
+    <t>create_PN_IP_Extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 90000000000000000001..90000000000000000010 -numbertype ex,extension -i -d 90000000000000000001..90000000000000000010 -l 1 --csp 0,ip_extension -i -d 90000000000000000001..90000000000000000010,90000000000000000001,90000000000000000002,90000000000000000003,90000000000000000004,90000000000000000005,90000000000000000006,90000000000000000007,90000000000000000008,90000000000000000009,90000000000000000010,ip_extension -e -d 90000000000000000001..90000000000000000010,extension -e -d 90000000000000000001..90000000000000000010,number_end -number 90000000000000000001..90000000000000000010 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,call_list -e -d 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-10-00,call_list -e -d 80000000000000000000,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>create_PN_Analog_Extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-2-20-00,call_list -e -d 80000000000000000000,KSEXE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>create_PN_Digital_Extension</t>
+  </si>
+  <si>
+    <t>create_PN_Virtual_Extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,call_list -e -d 80000000000000000000,extension -e -d 80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_create_PN_SIPDECT_Extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,Arjuna,99999,1104100450968,call_list -e -d 80000000000000000000,parallel_ringing -e --dir 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_IP_extension_assign_PN</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,extension -i -d 80000000000000000000 -l 1 --csp 0,ip_extension -i -d 80000000000000000000,call_list -e -d 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_Analog_extension_assign_PN</t>
+  </si>
+  <si>
+    <t>test_edit_Digital_extension_assign_PN</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,extension -i -d 80000000000000000000 -l 1 --csp 0,call_list -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_Virtual_extension_assign_PN</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1,Arjuna,99999,1104100450968,FirstName,LastName,call_list -e -d 80000000000000000000,parallel_ringing -e --dir 80000000000000000000,ip_extension -e -d 80000000000000000000,extension -e -d 80000000000000000000,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_edit_SIPDECT_Assign_PN</t>
   </si>
 </sst>
 </file>
@@ -935,7 +1044,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,7 +1069,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1004,7 +1113,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1015,7 +1124,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1026,7 +1135,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1037,7 +1146,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1051,17 +1160,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="48.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.08984375" customWidth="1"/>
-    <col min="4" max="4" width="76.1796875" customWidth="1"/>
+    <col min="4" max="4" width="76.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1091,7 +1200,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1099,7 +1208,7 @@
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -1110,7 +1219,7 @@
     </row>
     <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -1121,7 +1230,7 @@
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
@@ -1132,7 +1241,7 @@
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -1143,7 +1252,7 @@
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
@@ -1154,7 +1263,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1162,7 +1271,7 @@
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
@@ -1173,7 +1282,7 @@
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -1184,10 +1293,10 @@
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1195,10 +1304,10 @@
     </row>
     <row r="13" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1206,10 +1315,10 @@
     </row>
     <row r="14" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1217,10 +1326,10 @@
     </row>
     <row r="15" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -1228,10 +1337,10 @@
     </row>
     <row r="16" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1239,10 +1348,10 @@
     </row>
     <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1250,10 +1359,10 @@
     </row>
     <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1261,10 +1370,10 @@
     </row>
     <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1272,10 +1381,10 @@
     </row>
     <row r="20" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1283,10 +1392,10 @@
     </row>
     <row r="21" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1294,10 +1403,10 @@
     </row>
     <row r="22" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1305,10 +1414,10 @@
     </row>
     <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1316,80 +1425,80 @@
     </row>
     <row r="24" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1398,10 +1507,10 @@
     </row>
     <row r="30" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1410,10 +1519,10 @@
     </row>
     <row r="31" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1422,10 +1531,10 @@
     </row>
     <row r="32" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1434,38 +1543,38 @@
     </row>
     <row r="33" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1474,10 +1583,10 @@
     </row>
     <row r="36" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1485,10 +1594,10 @@
     </row>
     <row r="37" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1496,10 +1605,10 @@
     </row>
     <row r="38" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -1507,10 +1616,10 @@
     </row>
     <row r="39" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -1518,10 +1627,10 @@
     </row>
     <row r="40" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1529,10 +1638,10 @@
     </row>
     <row r="41" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1540,10 +1649,10 @@
     </row>
     <row r="42" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -1551,10 +1660,10 @@
     </row>
     <row r="43" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -1562,10 +1671,10 @@
     </row>
     <row r="44" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -1573,10 +1682,10 @@
     </row>
     <row r="45" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -1584,10 +1693,10 @@
     </row>
     <row r="46" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -1595,7 +1704,7 @@
     </row>
     <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>12</v>
@@ -1604,12 +1713,12 @@
         <v>4</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>12</v>
@@ -1618,12 +1727,12 @@
         <v>4</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>12</v>
@@ -1632,12 +1741,12 @@
         <v>4</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>12</v>
@@ -1646,29 +1755,29 @@
         <v>4</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -1676,24 +1785,24 @@
     </row>
     <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
@@ -1701,10 +1810,10 @@
     </row>
     <row r="55" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -1712,10 +1821,10 @@
     </row>
     <row r="56" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -1723,10 +1832,10 @@
     </row>
     <row r="57" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -1734,10 +1843,10 @@
     </row>
     <row r="58" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -1746,38 +1855,38 @@
     </row>
     <row r="59" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -1785,10 +1894,10 @@
     </row>
     <row r="62" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -1796,10 +1905,10 @@
     </row>
     <row r="63" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -1807,7 +1916,7 @@
     </row>
     <row r="64" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>12</v>
@@ -1816,12 +1925,12 @@
         <v>4</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>12</v>
@@ -1830,12 +1939,12 @@
         <v>4</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>12</v>
@@ -1844,12 +1953,12 @@
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>12</v>
@@ -1858,12 +1967,12 @@
         <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>12</v>
@@ -1872,12 +1981,12 @@
         <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>12</v>
@@ -1886,15 +1995,15 @@
         <v>4</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -1902,10 +2011,10 @@
     </row>
     <row r="71" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
@@ -1913,10 +2022,10 @@
     </row>
     <row r="72" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
@@ -1924,10 +2033,10 @@
     </row>
     <row r="73" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -1935,38 +2044,38 @@
     </row>
     <row r="74" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C75" t="s">
         <v>4</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C76" t="s">
         <v>4</v>
@@ -1974,10 +2083,10 @@
     </row>
     <row r="77" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
@@ -1985,10 +2094,10 @@
     </row>
     <row r="78" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>
@@ -1996,7 +2105,7 @@
     </row>
     <row r="79" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>12</v>
@@ -2005,12 +2114,12 @@
         <v>4</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>12</v>
@@ -2019,12 +2128,12 @@
         <v>4</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>12</v>
@@ -2033,12 +2142,12 @@
         <v>4</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>12</v>
@@ -2047,12 +2156,12 @@
         <v>4</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>12</v>
@@ -2061,12 +2170,12 @@
         <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>12</v>
@@ -2075,15 +2184,15 @@
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C85" t="s">
         <v>4</v>
@@ -2091,10 +2200,10 @@
     </row>
     <row r="86" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -2102,10 +2211,10 @@
     </row>
     <row r="87" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C87" t="s">
         <v>4</v>
@@ -2113,10 +2222,10 @@
     </row>
     <row r="88" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -2124,10 +2233,10 @@
     </row>
     <row r="89" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C89" t="s">
         <v>4</v>
@@ -2135,10 +2244,10 @@
     </row>
     <row r="90" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C90" t="s">
         <v>4</v>
@@ -2146,10 +2255,10 @@
     </row>
     <row r="91" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C91" t="s">
         <v>4</v>
@@ -2157,10 +2266,10 @@
     </row>
     <row r="92" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C92" t="s">
         <v>4</v>
@@ -2168,7 +2277,7 @@
     </row>
     <row r="93" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>12</v>
@@ -2177,12 +2286,12 @@
         <v>4</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>12</v>
@@ -2191,12 +2300,12 @@
         <v>4</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>12</v>
@@ -2205,12 +2314,12 @@
         <v>4</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>12</v>
@@ -2219,12 +2328,12 @@
         <v>4</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>12</v>
@@ -2233,12 +2342,12 @@
         <v>4</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>12</v>
@@ -2247,15 +2356,15 @@
         <v>4</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C99" t="s">
         <v>4</v>
@@ -2263,10 +2372,10 @@
     </row>
     <row r="100" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C100" t="s">
         <v>4</v>
@@ -2274,10 +2383,10 @@
     </row>
     <row r="101" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C101" t="s">
         <v>4</v>
@@ -2285,13 +2394,306 @@
     </row>
     <row r="102" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C102" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>190</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>192</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>193</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>194</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>196</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>199</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C108" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>200</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>201</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" t="s">
+        <v>4</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>202</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>203</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>204</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>205</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" t="s">
+        <v>4</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>206</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C115" t="s">
+        <v>4</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>210</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C116" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>212</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C117" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>213</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C118" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>215</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C119" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>217</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C120" t="s">
+        <v>4</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>219</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C121" t="s">
+        <v>4</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>220</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C122" t="s">
+        <v>4</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C123" t="s">
+        <v>4</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>224</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C124" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2341,7 +2743,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2351,12 +2753,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added jcommander and testng.jar fles to PM project...!
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C654562-4512-4F97-91CA-F7455D3B761D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8274D998-33AA-464C-AA0F-143D81E12125}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
@@ -705,16 +705,16 @@
     <t>test_edit_SIPDECT_Assign_PN</t>
   </si>
   <si>
-    <t>https://10.211.62.208/mp</t>
-  </si>
-  <si>
-    <t>https://10.211.62.208/wbm</t>
-  </si>
-  <si>
-    <t>rcg,Insp!re1</t>
-  </si>
-  <si>
     <t>number_initiate -number 80000000000000000000 -numbertype ex,80000000000000000000,1B-0-20-31,call_list -e -d 80000000000000000000,EXTEE:DIR=80000000000000000000;,number_end -number 80000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>https://10.211.62.214/wbm</t>
+  </si>
+  <si>
+    <t>https://10.211.62.216/mp</t>
+  </si>
+  <si>
+    <t>Arjuna,Arjuna@12345</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1072,7 +1072,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1165,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1705,7 +1705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>207</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
@@ -2746,7 +2746,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2756,7 +2756,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added bulk user Import script
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1FAE32-A0A5-440B-BE50-E675AFDBAD2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98673235-2BAC-47D3-BE79-73AD1C090549}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="236">
   <si>
     <t>TestCase</t>
   </si>
@@ -738,6 +738,12 @@
   </si>
   <si>
     <t>number_initiate -number 10000..10001 -numbertype ex##extension -i -d 10000..10001 -l 1 --csp 0##ip_extension -i -d 10000..10001##extension_key -i -d 10000 --function tns --display-text "TNS-10001" --key 1 --key-sequence 10001##10000##10001##extension_key -e -d 10000 --key 1##ip_extension -e -d 10000..10001##extension -e -d 10000..10001##number_end -number 10000..10001 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_bulk_user_import_with_existing_extensions</t>
+  </si>
+  <si>
+    <t>number_initiate -number 80000000000000000001..80000000000000001000 -numbertype ex##extension -i -d 80000000000000000001..80000000000000001000 -l 1 --csp 0##ip_extension -i -d 80000000000000000001..80000000000000001000##80000000000000000001##BulkUser##ip_extension -e -d 80000000000000000001..80000000000000001000##extension -e -d 80000000000000000001..80000000000000001000##number_end -number 80000000000000000001..80000000000000001000 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -1186,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1784,7 +1790,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -1982,7 +1988,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -2235,7 +2241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -2268,7 +2274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -2301,7 +2307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>107</v>
       </c>
@@ -2329,7 +2335,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>108</v>
       </c>
@@ -2343,7 +2349,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>109</v>
       </c>
@@ -2357,7 +2363,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>110</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>111</v>
       </c>
@@ -2790,6 +2796,17 @@
       </c>
       <c r="D129" s="2" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>234</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C130" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test scripts for numberSeries.
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4DA206-4049-4C7F-B3D7-85D537777279}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF988FF-DC24-4DED-8623-7D6B3D5559FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="327">
   <si>
     <t>TestCase</t>
   </si>
@@ -442,12 +442,6 @@
   </si>
   <si>
     <t>test_edit_SIPDECT_Assign_PN</t>
-  </si>
-  <si>
-    <t>https://10.211.62.214/wbm</t>
-  </si>
-  <si>
-    <t>https://10.211.62.216/mp</t>
   </si>
   <si>
     <t>edit_IP_extension_to_change_active_call_list</t>
@@ -885,6 +879,144 @@
   </si>
   <si>
     <t>test_edit_micollab_Role_from_premium_to_standard</t>
+  </si>
+  <si>
+    <t>http://10.211.62.216/mp</t>
+  </si>
+  <si>
+    <t>http://10.211.62.214/wbm</t>
+  </si>
+  <si>
+    <t>test_create_directoryNumbers</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Directory numbers##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Common operator numbers##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_commonOperatorNumbers</t>
+  </si>
+  <si>
+    <t>test_create_individualOperatorNumbers</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Individual operator numbers##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Common abbreviated numbers##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_commonAbbreviatedNumbers</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Emergency numbers to operator##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_emergencyOperatorNumbers</t>
+  </si>
+  <si>
+    <t>test_create_individualAbbreviatedNumbers</t>
+  </si>
+  <si>
+    <t>1,9##Individual abbreviated numbers##1##9</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Route directory numbers##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_routeDirectoryNumbers</t>
+  </si>
+  <si>
+    <t>test_create_dialedNumberInfoService</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Dialed number information service##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_pagingNumbers</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Paging numbers##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_gatewayRoutingNumbers</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Gateway routing numbers##90000000000000000000-90000000000000000099##pu_add -unit IGWP</t>
+  </si>
+  <si>
+    <t>9000000000,9000000001,9000000002-9000000099##External coordinated destination##9000000000-9000000099</t>
+  </si>
+  <si>
+    <t>test_create_externalCoordinatedNumbers</t>
+  </si>
+  <si>
+    <t>test_create_externalDestinationNumbers</t>
+  </si>
+  <si>
+    <t>9000000000,9000000001,9000000002-9000000099##External destination##9000000000-9000000099</t>
+  </si>
+  <si>
+    <t>test_create_leastCostRoutingAccessNumbers</t>
+  </si>
+  <si>
+    <t>9000000000,9000000001,9000000002-9000000099##Least cost routing access numbers##9000000000-9000000099</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Common direct in-dialing operator numbers##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_commonDirectInDialingOperatorNumbers</t>
+  </si>
+  <si>
+    <t>test_create_ownNodeNumbers</t>
+  </si>
+  <si>
+    <t>90000,90001,90002-90099##Own node number##90000-90099</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001##Common public directory numbers##90000000000000000000##90000000000000000001</t>
+  </si>
+  <si>
+    <t>test_create_commonPublicDirectoryNumbers</t>
+  </si>
+  <si>
+    <t>test_create_accessNumbersForMobExtWithOutAuth</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Access numbers for mobile extension (without authorization)##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Access numbers for mobile extension (with authorization)##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_accessNumbersForMobExtWithAuth</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Access numbers for mobile extension (without authorization and DialTone)##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>test_create_accessNumbersForMobExtWithOutAuthAndDialTone</t>
+  </si>
+  <si>
+    <t>9000000000,9000000001,9000000002-9000000099##Public destination least cost routing##9000000000-9000000099</t>
+  </si>
+  <si>
+    <t>test_create_publicDestLeastCostRouting</t>
+  </si>
+  <si>
+    <t>test_create_directInwardServiceAccess</t>
+  </si>
+  <si>
+    <t>90000000000000000000,90000000000000000001,90000000000000000002-90000000000000000099##Direct inward service access##90000000000000000000-90000000000000000099</t>
+  </si>
+  <si>
+    <t>9000000000,9000000001,9000000002-9000000099##Fictitious destination numbers##9000000000-9000000099</t>
+  </si>
+  <si>
+    <t>test_create_fictiousDestNumbers</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1349,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1242,7 +1374,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1264,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1275,7 +1407,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1286,7 +1418,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1308,7 +1440,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1319,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1327,10 +1459,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1346,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1374,7 +1506,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1385,7 +1517,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1396,7 +1528,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1407,7 +1539,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1418,7 +1550,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1429,7 +1561,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1440,7 +1572,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1459,40 +1591,40 @@
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1503,29 +1635,29 @@
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1536,18 +1668,18 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1558,7 +1690,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1569,7 +1701,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1580,18 +1712,18 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1602,7 +1734,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1613,13 +1745,13 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -1627,13 +1759,13 @@
         <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -1641,13 +1773,13 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -1655,13 +1787,13 @@
         <v>39</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -1669,13 +1801,13 @@
         <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -1683,7 +1815,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1695,7 +1827,7 @@
         <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1707,7 +1839,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1719,7 +1851,7 @@
         <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1731,7 +1863,7 @@
         <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -1745,7 +1877,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -1759,7 +1891,7 @@
         <v>48</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1771,7 +1903,7 @@
         <v>49</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1782,7 +1914,7 @@
         <v>50</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1793,7 +1925,7 @@
         <v>51</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -1804,7 +1936,7 @@
         <v>52</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -1815,7 +1947,7 @@
         <v>53</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1826,7 +1958,7 @@
         <v>54</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1837,7 +1969,7 @@
         <v>55</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -1848,7 +1980,7 @@
         <v>56</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -1859,7 +1991,7 @@
         <v>57</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -1870,7 +2002,7 @@
         <v>58</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -1881,7 +2013,7 @@
         <v>59</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -1892,27 +2024,27 @@
         <v>60</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>61</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1920,13 +2052,13 @@
         <v>62</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1934,13 +2066,13 @@
         <v>63</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1948,13 +2080,13 @@
         <v>64</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -1962,7 +2094,7 @@
         <v>65</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -1973,13 +2105,13 @@
         <v>66</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
         <v>4</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -1987,7 +2119,7 @@
         <v>68</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
@@ -1998,7 +2130,7 @@
         <v>69</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -2009,7 +2141,7 @@
         <v>70</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -2020,7 +2152,7 @@
         <v>71</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -2031,7 +2163,7 @@
         <v>72</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -2043,13 +2175,13 @@
         <v>73</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="116" x14ac:dyDescent="0.35">
@@ -2057,13 +2189,13 @@
         <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2071,7 +2203,7 @@
         <v>75</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -2082,7 +2214,7 @@
         <v>76</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -2093,7 +2225,7 @@
         <v>77</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -2104,13 +2236,13 @@
         <v>78</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2118,13 +2250,13 @@
         <v>79</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C65" t="s">
         <v>4</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2132,13 +2264,13 @@
         <v>80</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2146,13 +2278,13 @@
         <v>81</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2160,13 +2292,13 @@
         <v>82</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2174,13 +2306,13 @@
         <v>83</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2188,7 +2320,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -2199,7 +2331,7 @@
         <v>84</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
@@ -2210,7 +2342,7 @@
         <v>85</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
@@ -2221,7 +2353,7 @@
         <v>86</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -2232,13 +2364,13 @@
         <v>87</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2246,13 +2378,13 @@
         <v>88</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C75" t="s">
         <v>4</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2260,7 +2392,7 @@
         <v>89</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C76" t="s">
         <v>4</v>
@@ -2271,7 +2403,7 @@
         <v>90</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
@@ -2282,7 +2414,7 @@
         <v>91</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>
@@ -2293,13 +2425,13 @@
         <v>92</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C79" t="s">
         <v>4</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2307,13 +2439,13 @@
         <v>93</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C80" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2321,13 +2453,13 @@
         <v>94</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2335,13 +2467,13 @@
         <v>95</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C82" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2349,13 +2481,13 @@
         <v>96</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C83" t="s">
         <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2363,13 +2495,13 @@
         <v>97</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C84" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2377,7 +2509,7 @@
         <v>98</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C85" t="s">
         <v>4</v>
@@ -2388,7 +2520,7 @@
         <v>99</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -2399,7 +2531,7 @@
         <v>100</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C87" t="s">
         <v>4</v>
@@ -2410,7 +2542,7 @@
         <v>101</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -2421,7 +2553,7 @@
         <v>102</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C89" t="s">
         <v>4</v>
@@ -2432,7 +2564,7 @@
         <v>103</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C90" t="s">
         <v>4</v>
@@ -2443,7 +2575,7 @@
         <v>104</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C91" t="s">
         <v>4</v>
@@ -2454,7 +2586,7 @@
         <v>105</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C92" t="s">
         <v>4</v>
@@ -2465,13 +2597,13 @@
         <v>106</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C93" t="s">
         <v>4</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2479,13 +2611,13 @@
         <v>107</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C94" t="s">
         <v>4</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2493,13 +2625,13 @@
         <v>108</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C95" t="s">
         <v>4</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2507,13 +2639,13 @@
         <v>109</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C96" t="s">
         <v>4</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2521,13 +2653,13 @@
         <v>110</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C97" t="s">
         <v>4</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2535,13 +2667,13 @@
         <v>111</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C98" t="s">
         <v>4</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2549,7 +2681,7 @@
         <v>112</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C99" t="s">
         <v>4</v>
@@ -2560,7 +2692,7 @@
         <v>113</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C100" t="s">
         <v>4</v>
@@ -2571,7 +2703,7 @@
         <v>114</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C101" t="s">
         <v>4</v>
@@ -2582,7 +2714,7 @@
         <v>115</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C102" t="s">
         <v>4</v>
@@ -2593,7 +2725,7 @@
         <v>116</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C103" t="s">
         <v>4</v>
@@ -2604,7 +2736,7 @@
         <v>117</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C104" t="s">
         <v>4</v>
@@ -2615,7 +2747,7 @@
         <v>118</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C105" t="s">
         <v>4</v>
@@ -2626,13 +2758,13 @@
         <v>119</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C106" t="s">
         <v>4</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -2640,7 +2772,7 @@
         <v>120</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C107" t="s">
         <v>4</v>
@@ -2651,13 +2783,13 @@
         <v>121</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C108" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C108" t="s">
-        <v>4</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -2665,7 +2797,7 @@
         <v>122</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C109" t="s">
         <v>4</v>
@@ -2676,13 +2808,13 @@
         <v>123</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C110" t="s">
         <v>4</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2690,13 +2822,13 @@
         <v>124</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C111" t="s">
         <v>4</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2704,13 +2836,13 @@
         <v>125</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C112" t="s">
         <v>4</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2718,13 +2850,13 @@
         <v>126</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C113" t="s">
         <v>4</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2732,13 +2864,13 @@
         <v>127</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C114" t="s">
         <v>4</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2746,13 +2878,13 @@
         <v>128</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C115" t="s">
         <v>4</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2760,13 +2892,13 @@
         <v>129</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2774,13 +2906,13 @@
         <v>130</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C117" t="s">
         <v>4</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2788,13 +2920,13 @@
         <v>131</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C118" t="s">
         <v>4</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2802,13 +2934,13 @@
         <v>132</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C119" t="s">
         <v>4</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2816,13 +2948,13 @@
         <v>133</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C120" t="s">
         <v>4</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2830,13 +2962,13 @@
         <v>134</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C121" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2844,13 +2976,13 @@
         <v>135</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C122" t="s">
         <v>4</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2858,13 +2990,13 @@
         <v>136</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C123" t="s">
         <v>4</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2872,91 +3004,91 @@
         <v>137</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C124" t="s">
         <v>4</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C125" t="s">
         <v>4</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C126" t="s">
         <v>4</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C127" t="s">
         <v>4</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C128" t="s">
         <v>4</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C129" t="s">
         <v>4</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C130" t="s">
         <v>4</v>
@@ -2964,10 +3096,10 @@
     </row>
     <row r="131" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C131" t="s">
         <v>4</v>
@@ -2975,10 +3107,10 @@
     </row>
     <row r="132" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C132" t="s">
         <v>4</v>
@@ -2986,10 +3118,10 @@
     </row>
     <row r="133" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C133" t="s">
         <v>4</v>
@@ -2997,10 +3129,10 @@
     </row>
     <row r="134" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C134" t="s">
         <v>4</v>
@@ -3008,10 +3140,10 @@
     </row>
     <row r="135" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C135" t="s">
         <v>4</v>
@@ -3019,359 +3151,359 @@
     </row>
     <row r="136" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C136" t="s">
         <v>4</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C137" t="s">
         <v>4</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C138" t="s">
         <v>4</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C139" t="s">
         <v>4</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C140" t="s">
         <v>4</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C141" t="s">
         <v>4</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C142" t="s">
         <v>4</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C143" t="s">
         <v>4</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C144" t="s">
         <v>4</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C145" t="s">
         <v>4</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C146" t="s">
         <v>4</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C147" t="s">
         <v>4</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C148" t="s">
         <v>4</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C149" t="s">
         <v>4</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C150" t="s">
         <v>4</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C151" t="s">
         <v>4</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C152" t="s">
         <v>4</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C153" t="s">
         <v>4</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C154" t="s">
         <v>4</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C155" t="s">
         <v>4</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C156" t="s">
         <v>4</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C157" t="s">
         <v>4</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C158" t="s">
         <v>4</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C159" t="s">
         <v>4</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3382,15 +3514,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB728E-D6A2-4728-8CDB-693BFA2A04D3}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="1" max="1" width="46.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3405,11 +3537,247 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
+    <row r="2" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="2"/>
+      <c r="A7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>307</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>311</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>315</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>320</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>322</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>323</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3421,7 +3789,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3431,17 +3799,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test cases for account code
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mallikarjuna\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2B29C8-9B4D-4A97-BA17-DD08E6945201}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFE8519-8A77-4FD1-9E1C-9981B1C35F00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="14400" windowHeight="7335" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="368">
   <si>
     <t>TestCase</t>
   </si>
@@ -1013,13 +1013,133 @@
     <t>test_create_fictiousDestNumbers</t>
   </si>
   <si>
-    <t>https://10.211.62.216/mp</t>
-  </si>
-  <si>
-    <t>https://10.211.62.214/wbm</t>
-  </si>
-  <si>
-    <t>SomeChanges</t>
+    <t>http://10.211.162.213/mp</t>
+  </si>
+  <si>
+    <t>http://10.211.162.213/wbm</t>
+  </si>
+  <si>
+    <t>test_create_external_number_length</t>
+  </si>
+  <si>
+    <t>9999999999##3##5</t>
+  </si>
+  <si>
+    <t>test_edit_extNumLength</t>
+  </si>
+  <si>
+    <t>9999999999##3##5##8888888888</t>
+  </si>
+  <si>
+    <t>test_verify_popup_when_num_greaterThanLen10</t>
+  </si>
+  <si>
+    <t>99999999999##3</t>
+  </si>
+  <si>
+    <t>test_verify_popup_when_minLenNum_greaterThanMaxLenNum</t>
+  </si>
+  <si>
+    <t>9999999999##5##3</t>
+  </si>
+  <si>
+    <t>test_create_extNumLength_without_minNumber</t>
+  </si>
+  <si>
+    <t>9999999999</t>
+  </si>
+  <si>
+    <t>test_edit_extNumLength_provide_minLength_greater_thanMaxLength</t>
+  </si>
+  <si>
+    <t>9999999999##3##4##5</t>
+  </si>
+  <si>
+    <t>test_create_account_code</t>
+  </si>
+  <si>
+    <t>999999999999999</t>
+  </si>
+  <si>
+    <t>9999999999999999</t>
+  </si>
+  <si>
+    <t>test_create_account_code_with_firstANDLastCodes</t>
+  </si>
+  <si>
+    <t>999999999999990##999999999999999##999999999999990 - 999999999999999</t>
+  </si>
+  <si>
+    <t>test_create_accountCode_moreThan_15_Digits</t>
+  </si>
+  <si>
+    <t>test_create_accountCodeFirst_moreThan_15_Digits</t>
+  </si>
+  <si>
+    <t>9999999999999999##999999999999990</t>
+  </si>
+  <si>
+    <t>test_create_accountCodeLast_moreThan_15_Digits</t>
+  </si>
+  <si>
+    <t>999999999999990##9999999999999999</t>
+  </si>
+  <si>
+    <t>test_verify_errMsg_when_accCode_First_last_are_provided</t>
+  </si>
+  <si>
+    <t>999999999999999##999999999999990##999999999999999</t>
+  </si>
+  <si>
+    <t>test_verify_errMsg_when_only_accCode_First_is_provided</t>
+  </si>
+  <si>
+    <t>test_verify_errMsg_when_only_accCode_Last_is_provided</t>
+  </si>
+  <si>
+    <t>test_create_account_code_withCustomer</t>
+  </si>
+  <si>
+    <t>999999999999999##Mitel##1</t>
+  </si>
+  <si>
+    <t>test_create_account_code_with_firstANDLastCodes_withCustomer</t>
+  </si>
+  <si>
+    <t>999999999999990##999999999999999##999999999999990 - 999999999999999##Mitel##1</t>
+  </si>
+  <si>
+    <t>9999999999999999##Mitel##1</t>
+  </si>
+  <si>
+    <t>test_create_accountCode_moreThan_15_Digits_withCustomer</t>
+  </si>
+  <si>
+    <t>9999999999999999##999999999999990##Mitel##1</t>
+  </si>
+  <si>
+    <t>test_create_accountCodeFirst_moreThan_15_Digits_withCustomer</t>
+  </si>
+  <si>
+    <t>999999999999990##9999999999999999##Mitel##1</t>
+  </si>
+  <si>
+    <t>test_create_accountCodeLast_moreThan_15_Digits_withCustomer</t>
+  </si>
+  <si>
+    <t>999999999999999##999999999999990##999999999999999##Mitel##1</t>
+  </si>
+  <si>
+    <t>test_verify_errMsg_when_accCode_First_last_are_provided_withCustomer</t>
+  </si>
+  <si>
+    <t>test_verify_errMsg_when_only_accCode_First_is_provided_withCustomer</t>
+  </si>
+  <si>
+    <t>test_verify_errMsg_when_only_accCode_Last_is_provided_withCustomer</t>
+  </si>
+  <si>
+    <t>test_delete_accountCode_using_delete_button</t>
   </si>
 </sst>
 </file>
@@ -1072,13 +1192,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3528,15 +3651,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB728E-D6A2-4728-8CDB-693BFA2A04D3}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3790,6 +3913,259 @@
         <v>323</v>
       </c>
       <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>329</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>335</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>337</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>339</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>342</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>344</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>345</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>347</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>349</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>351</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>352</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>353</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>355</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>358</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>360</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>362</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>364</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>365</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>366</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>367</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C46" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3800,10 +4176,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E53A9E-ACD5-46DD-9427-7F06AD780F15}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3826,11 +4202,6 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>327</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{4A8B273B-2866-46CE-9E3B-FE96A3A17BA9}"/>

</xml_diff>

<commit_message>
added CSP Test Case
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mallikarjuna\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFE8519-8A77-4FD1-9E1C-9981B1C35F00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC224FC4-4910-4CBD-98D7-388DFCB7B437}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="370">
   <si>
     <t>TestCase</t>
   </si>
@@ -1140,6 +1140,12 @@
   </si>
   <si>
     <t>test_delete_accountCode_using_delete_button</t>
+  </si>
+  <si>
+    <t>test_create_CSP</t>
+  </si>
+  <si>
+    <t>CSP 1</t>
   </si>
 </sst>
 </file>
@@ -1615,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3651,10 +3657,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB728E-D6A2-4728-8CDB-693BFA2A04D3}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,6 +4172,17 @@
         <v>340</v>
       </c>
       <c r="C46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>368</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C47" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added common CAT Test Cases
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mallikarjuna\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3833488-4716-4B9B-9512-73FF10CB4A46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8767DF-1DF7-4564-A371-7DF9E25EC3C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="398">
   <si>
     <t>TestCase</t>
   </si>
@@ -1142,9 +1142,6 @@
     <t>http://10.211.162.111/mp</t>
   </si>
   <si>
-    <t>http://10.211.162.111/wbm</t>
-  </si>
-  <si>
     <t>test_create_default_CSP</t>
   </si>
   <si>
@@ -1224,6 +1221,15 @@
   </si>
   <si>
     <t>CSP2##EditedCSP</t>
+  </si>
+  <si>
+    <t>test_create_CAT</t>
+  </si>
+  <si>
+    <t>https://10.211.62.214/wbm</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1576,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3735,10 +3741,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB728E-D6A2-4728-8CDB-693BFA2A04D3}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4258,7 +4264,7 @@
         <v>366</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -4266,10 +4272,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
@@ -4277,10 +4283,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
@@ -4288,10 +4294,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -4299,10 +4305,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -4310,10 +4316,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -4321,10 +4327,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C53" t="s">
         <v>4</v>
@@ -4332,10 +4338,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
@@ -4343,10 +4349,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -4354,10 +4360,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -4365,10 +4371,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -4376,10 +4382,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -4387,10 +4393,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
@@ -4398,10 +4404,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>383</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -4409,10 +4415,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>385</v>
+      </c>
+      <c r="B61" t="s">
         <v>386</v>
-      </c>
-      <c r="B61" t="s">
-        <v>387</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -4420,10 +4426,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>387</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -4431,10 +4437,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>389</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -4442,10 +4448,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>391</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>393</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
@@ -4453,12 +4459,23 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>393</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>395</v>
       </c>
-      <c r="C65" t="s">
+      <c r="B66" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C66" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4472,7 +4489,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4487,7 +4504,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>368</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added configurations in Base Class
</commit_message>
<xml_diff>
--- a/PM/src/main/java/myTestData/TestData.xlsx
+++ b/PM/src/main/java/myTestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mallikarjuna\git\PM\PM\src\main\java\myTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B37EBA-8A54-449A-94C3-B48C8E30A4E4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4DFEB8-D63E-41E5-A358-0FFE86CC4619}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,30 +1011,6 @@
     <t>number_initiate -number 80000000000000000000 -numbertype ex##80000000000000000000##1##Arjuna##99999##1034503032509##FirstName##LastName##call_list -e -d 80000000000000000000##parallel_ringing -e --dir 80000000000000000000##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
   </si>
   <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##80000000000000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##Basic User##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##80000000000000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##UCC (V4.0) Entry##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##80000000000000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##UCC (V4.0) Standard##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##80000000000000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##UCC (V4.0) Premium##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##extension -i -d 80000000000000000000 -l 1 --csp 0##ip_extension -i -d 80000000000000000000##auth_code -i --dir 80000000000000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##80000000000000000000##UCC (V4.0) Premium##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##extension -i -d 80000000000000000000 -l 1 --csp 0##ip_extension -i -d 80000000000000000000##auth_code -i --dir 80000000000000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##80000000000000000000##UCC (V4.0) Standard##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##extension -i -d 80000000000000000000 -l 1 --csp 0##ip_extension -i -d 80000000000000000000##auth_code -i --dir 80000000000000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##80000000000000000000##UCC (V4.0) Entry##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
-    <t>number_initiate -number 80000000000000000000 -numbertype ex##extension -i -d 80000000000000000000 -l 1 --csp 0##ip_extension -i -d 80000000000000000000##auth_code -i --dir 80000000000000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##80000000000000000000##Basic User##ip_extension -e -d 80000000000000000000##extension -e -d 80000000000000000000##number_end -number 80000000000000000000 -numbertype ex</t>
-  </si>
-  <si>
     <t>number_initiate -number 10000000000000000001 -numbertype ex##10000000000000000001##10000000000000000001##1##FirstName##LastName##Mitel 6869i##ip_extension -e -d 10000000000000000001##extension -e -d 10000000000000000001##number_end -number 10000000000000000001 -numbertype ex</t>
   </si>
   <si>
@@ -1239,6 +1215,30 @@
   </si>
   <si>
     <t>number_initiate -number 90000000000000000000 -numbertype ex##extension -i -d 90000000000000000000 -l 1 --csp 0##ip_extension -i -d 90000000000000000000##90000000000000000000##ip_extension -e -d 90000000000000000000##extension -e -d 90000000000000000000##number_end -number 90000000000000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##8000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##Basic User##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##8000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##UCC (V4.0) Entry##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##8000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##UCC (V4.0) Standard##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##8000000000##FirstName##LastName##Mitel 6869i##1234567890##CLEARTEXT##UCC (V4.0) Premium##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##extension -i -d 8000000000 -l 1 --csp 0##ip_extension -i -d 8000000000##auth_code -i --dir 8000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##8000000000##UCC (V4.0) Premium##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##extension -i -d 8000000000 -l 1 --csp 0##ip_extension -i -d 8000000000##auth_code -i --dir 8000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##8000000000##UCC (V4.0) Standard##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##extension -i -d 8000000000 -l 1 --csp 0##ip_extension -i -d 8000000000##auth_code -i --dir 8000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##8000000000##UCC (V4.0) Entry##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
+  </si>
+  <si>
+    <t>number_initiate -number 8000000000 -numbertype ex##extension -i -d 8000000000 -l 1 --csp 0##ip_extension -i -d 8000000000##auth_code -i --dir 8000000000 --auth-code 1234567890 --hash-type CLEARTEXT --cil 1234567890 --csp 0##8000000000##Basic User##ip_extension -e -d 8000000000##extension -e -d 8000000000##number_end -number 8000000000 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1299,6 +1299,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1718,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F58A62-9022-4E18-A958-558EAA09A02C}">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1875,7 +1878,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1886,7 +1889,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -1897,7 +1900,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1908,7 +1911,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1919,7 +1922,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1930,7 +1933,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1941,7 +1944,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1952,7 +1955,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1963,7 +1966,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1974,7 +1977,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1985,13 +1988,13 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -1999,13 +2002,13 @@
         <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2013,13 +2016,13 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2027,13 +2030,13 @@
         <v>39</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -2041,13 +2044,13 @@
         <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -2055,7 +2058,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -2067,7 +2070,7 @@
         <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -2079,7 +2082,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -2091,7 +2094,7 @@
         <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2103,13 +2106,13 @@
         <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
@@ -2117,13 +2120,13 @@
         <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="203" x14ac:dyDescent="0.35">
@@ -2131,7 +2134,7 @@
         <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -2143,7 +2146,7 @@
         <v>48</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -2154,7 +2157,7 @@
         <v>49</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -2165,7 +2168,7 @@
         <v>50</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -2176,7 +2179,7 @@
         <v>51</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -2187,7 +2190,7 @@
         <v>52</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -2198,7 +2201,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -2209,7 +2212,7 @@
         <v>54</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -2220,7 +2223,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -2231,7 +2234,7 @@
         <v>56</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -2242,7 +2245,7 @@
         <v>57</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -2253,7 +2256,7 @@
         <v>58</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -2270,7 +2273,7 @@
         <v>4</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2298,7 +2301,7 @@
         <v>4</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2312,7 +2315,7 @@
         <v>4</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2326,7 +2329,7 @@
         <v>4</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2351,7 +2354,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2359,7 +2362,7 @@
         <v>67</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
@@ -2370,7 +2373,7 @@
         <v>68</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -2381,7 +2384,7 @@
         <v>69</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -2392,7 +2395,7 @@
         <v>70</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -2403,7 +2406,7 @@
         <v>71</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -2415,13 +2418,13 @@
         <v>72</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="116" x14ac:dyDescent="0.35">
@@ -2429,13 +2432,13 @@
         <v>73</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2443,7 +2446,7 @@
         <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -2454,7 +2457,7 @@
         <v>75</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -2465,7 +2468,7 @@
         <v>76</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -2482,7 +2485,7 @@
         <v>4</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2496,7 +2499,7 @@
         <v>4</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2510,7 +2513,7 @@
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2524,7 +2527,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2538,7 +2541,7 @@
         <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2552,7 +2555,7 @@
         <v>4</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2560,7 +2563,7 @@
         <v>66</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -2571,7 +2574,7 @@
         <v>83</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
@@ -2582,7 +2585,7 @@
         <v>84</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
@@ -2593,7 +2596,7 @@
         <v>85</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -2604,13 +2607,13 @@
         <v>86</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -2618,13 +2621,13 @@
         <v>87</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C75" t="s">
         <v>4</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2632,7 +2635,7 @@
         <v>88</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C76" t="s">
         <v>4</v>
@@ -2643,7 +2646,7 @@
         <v>89</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
@@ -2654,7 +2657,7 @@
         <v>90</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>
@@ -2671,7 +2674,7 @@
         <v>4</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2685,7 +2688,7 @@
         <v>4</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2699,7 +2702,7 @@
         <v>4</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2713,7 +2716,7 @@
         <v>4</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2727,7 +2730,7 @@
         <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2741,7 +2744,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -2771,7 +2774,7 @@
         <v>99</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C87" t="s">
         <v>4</v>
@@ -2782,7 +2785,7 @@
         <v>100</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -2804,7 +2807,7 @@
         <v>102</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C90" t="s">
         <v>4</v>
@@ -3004,7 +3007,7 @@
         <v>4</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -3029,7 +3032,7 @@
         <v>4</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -3124,7 +3127,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3132,13 +3135,13 @@
         <v>128</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3146,13 +3149,13 @@
         <v>129</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C117" t="s">
         <v>4</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3166,7 +3169,7 @@
         <v>4</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3180,7 +3183,7 @@
         <v>4</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3194,7 +3197,7 @@
         <v>4</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3202,13 +3205,13 @@
         <v>133</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="C121" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3216,13 +3219,13 @@
         <v>134</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C122" t="s">
         <v>4</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3236,7 +3239,7 @@
         <v>4</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3250,7 +3253,7 @@
         <v>4</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3264,7 +3267,7 @@
         <v>4</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3272,13 +3275,13 @@
         <v>138</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="C126" t="s">
         <v>4</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3286,13 +3289,13 @@
         <v>139</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C127" t="s">
         <v>4</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -3306,7 +3309,7 @@
         <v>4</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="174" x14ac:dyDescent="0.35">
@@ -3320,7 +3323,7 @@
         <v>4</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="174" x14ac:dyDescent="0.35">
@@ -3328,7 +3331,7 @@
         <v>149</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C130" t="s">
         <v>4</v>
@@ -3339,7 +3342,7 @@
         <v>150</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C131" t="s">
         <v>4</v>
@@ -3350,7 +3353,7 @@
         <v>151</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="C132" t="s">
         <v>4</v>
@@ -3361,7 +3364,7 @@
         <v>152</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="C133" t="s">
         <v>4</v>
@@ -3372,7 +3375,7 @@
         <v>153</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C134" t="s">
         <v>4</v>
@@ -3383,7 +3386,7 @@
         <v>154</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C135" t="s">
         <v>4</v>
@@ -3393,14 +3396,14 @@
       <c r="A136" t="s">
         <v>159</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="5" t="s">
         <v>158</v>
       </c>
       <c r="C136" t="s">
         <v>4</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>324</v>
+        <v>391</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3414,7 +3417,7 @@
         <v>4</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3428,7 +3431,7 @@
         <v>4</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>326</v>
+        <v>393</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3442,7 +3445,7 @@
         <v>4</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>327</v>
+        <v>394</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
@@ -3456,7 +3459,7 @@
         <v>4</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>328</v>
+        <v>395</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
@@ -3470,7 +3473,7 @@
         <v>4</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>329</v>
+        <v>396</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
@@ -3484,7 +3487,7 @@
         <v>4</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>330</v>
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
@@ -3498,7 +3501,7 @@
         <v>4</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>331</v>
+        <v>398</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3512,7 +3515,7 @@
         <v>4</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>324</v>
+        <v>391</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>167</v>
@@ -3529,7 +3532,7 @@
         <v>4</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>167</v>
@@ -3546,7 +3549,7 @@
         <v>4</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>327</v>
+        <v>394</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>167</v>
@@ -3563,7 +3566,7 @@
         <v>4</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>326</v>
+        <v>393</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>167</v>
@@ -3580,7 +3583,7 @@
         <v>4</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>324</v>
+        <v>391</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>167</v>
@@ -3597,7 +3600,7 @@
         <v>4</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>324</v>
+        <v>391</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>167</v>
@@ -3614,7 +3617,7 @@
         <v>4</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>324</v>
+        <v>391</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>167</v>
@@ -3631,7 +3634,7 @@
         <v>4</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3645,7 +3648,7 @@
         <v>4</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3659,7 +3662,7 @@
         <v>4</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>325</v>
+        <v>392</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3673,7 +3676,7 @@
         <v>4</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>326</v>
+        <v>393</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3687,7 +3690,7 @@
         <v>4</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>326</v>
+        <v>393</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3701,7 +3704,7 @@
         <v>4</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>326</v>
+        <v>393</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3715,7 +3718,7 @@
         <v>4</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>327</v>
+        <v>394</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3729,7 +3732,7 @@
         <v>4</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>327</v>
+        <v>394</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -3743,12 +3746,15 @@
         <v>4</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>327</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B136" r:id="rId1" xr:uid="{35C0A96E-4232-49F2-82A0-076A45945ECB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3757,7 +3763,7 @@
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4513,7 +4519,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>